<commit_message>
data and new stimuli videos
</commit_message>
<xml_diff>
--- a/data/LittleDrummers_FormattedDataSheet.xlsx
+++ b/data/LittleDrummers_FormattedDataSheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goldsmithscollege-my.sharepoint.com/personal/caddy001_campus_goldsmiths_ac_uk/Documents/Projects/Little Drummers/little-drummers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4586" documentId="13_ncr:1_{53DFB0FB-E263-4462-AC16-1659549806B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5415A8-E4B5-418D-AE74-54F18D263CD2}"/>
+  <xr:revisionPtr revIDLastSave="4590" documentId="13_ncr:1_{53DFB0FB-E263-4462-AC16-1659549806B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA9C8132-D30D-4D99-B228-B8349AEEAAD8}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="900" windowWidth="28830" windowHeight="12285" xr2:uid="{E658CBCD-6072-4503-AB93-02DC05FF206C}"/>
+    <workbookView xWindow="4155" yWindow="4365" windowWidth="28830" windowHeight="12285" activeTab="4" xr2:uid="{E658CBCD-6072-4503-AB93-02DC05FF206C}"/>
   </bookViews>
   <sheets>
     <sheet name="ManualCoding" sheetId="1" r:id="rId1"/>
     <sheet name="Fourier.All.0.5Hzcuttoff" sheetId="4" r:id="rId2"/>
     <sheet name="Fourier.All.1.0Hzcuttoff" sheetId="6" r:id="rId3"/>
     <sheet name="Drumming.Accuracy" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6211" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6261" uniqueCount="1080">
   <si>
     <t>ChildID</t>
   </si>
@@ -3308,7 +3309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3378,6 +3379,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3700,7 +3707,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3938,6 +3945,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -4278,11 +4288,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D932A98A-6DD1-4F28-B61A-6D2E2301002B}">
   <dimension ref="A1:IJ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82225,7 +82235,7 @@
   <dimension ref="A1:K209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K209"/>
+      <selection activeCell="B209" sqref="B2:B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88585,4 +88595,288 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95500FE2-4A1A-4481-9950-C1ACD8A26AD7}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D6" s="89">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D7" s="89">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D8" s="89">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D9" s="89">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D10" s="89">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D11" s="89">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>